<commit_message>
Added API validation (few assertions missing)
</commit_message>
<xml_diff>
--- a/data/qaautomation.xlsx
+++ b/data/qaautomation.xlsx
@@ -508,10 +508,10 @@
         <v>201</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
@@ -525,7 +525,7 @@
         <v xml:space="preserve">{
     "first_name": "Ali",
     "last_name": "Ahmad",
-    "email": "ali.ahmad23@gmail.com",
+    "email": "ali.ahmad2131@gmail.com",
     "password": "12345",
     "confirm_password": "12345"
 }</v>
@@ -537,7 +537,7 @@
         <v>200</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1">
         <v>2</v>
@@ -563,7 +563,7 @@
         <v>200</v>
       </c>
       <c r="F4" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
Created script to run test sequentially
</commit_message>
<xml_diff>
--- a/data/qaautomation.xlsx
+++ b/data/qaautomation.xlsx
@@ -61,136 +61,13 @@
     <t xml:space="preserve">After Life (TV Series 2019– ) - IMDb</t>
   </si>
   <si>
-    <t xml:space="preserve">tony.way52@gmail.com</t>
+    <t xml:space="preserve">tony.way53@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Emumba Pvt. Limited, Korang Road I-10/3 Islamabad.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">hello there</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">covid-19</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">zara hut k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">]</t>
-    </r>
+    <t xml:space="preserve">["hello there","covid-19","zara hut k"]</t>
   </si>
   <si>
     <t xml:space="preserve">API</t>
@@ -734,7 +611,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -756,12 +633,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -838,20 +709,13 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="35.7"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -931,15 +795,12 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="67.37"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -962,7 +823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -985,7 +846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1008,7 +869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1056,16 +917,16 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -1076,7 +937,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1087,7 +948,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -1098,7 +959,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -1109,7 +970,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1120,7 +981,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
@@ -1131,7 +992,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1142,7 +1003,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -1153,7 +1014,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -1164,7 +1025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1175,7 +1036,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -1186,7 +1047,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -1197,7 +1058,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1208,7 +1069,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1219,7 +1080,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1230,7 +1091,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1266,12 +1127,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.39"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1282,7 +1140,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -1293,7 +1151,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -1304,7 +1162,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1315,7 +1173,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1326,7 +1184,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
@@ -1337,7 +1195,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>63</v>
       </c>
@@ -1348,7 +1206,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
@@ -1359,7 +1217,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
@@ -1370,7 +1228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
@@ -1381,7 +1239,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>71</v>
       </c>
@@ -1392,7 +1250,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
@@ -1403,7 +1261,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1414,7 +1272,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -1425,7 +1283,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>80</v>
       </c>
@@ -1436,7 +1294,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>83</v>
       </c>
@@ -1447,7 +1305,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -1458,7 +1316,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -1469,7 +1327,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>90</v>
       </c>
@@ -1480,7 +1338,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>93</v>
       </c>
@@ -1491,7 +1349,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
@@ -1502,7 +1360,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>99</v>
       </c>
@@ -1513,7 +1371,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>102</v>
       </c>
@@ -1524,7 +1382,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>105</v>
       </c>
@@ -1535,7 +1393,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
@@ -1546,7 +1404,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>110</v>
       </c>
@@ -1557,7 +1415,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>113</v>
       </c>
@@ -1568,7 +1426,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>116</v>
       </c>
@@ -1579,7 +1437,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>119</v>
       </c>
@@ -1590,7 +1448,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>122</v>
       </c>
@@ -1601,7 +1459,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>124</v>
       </c>
@@ -1612,7 +1470,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>126</v>
       </c>
@@ -1623,7 +1481,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>128</v>
       </c>
@@ -1634,7 +1492,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>130</v>
       </c>
@@ -1645,7 +1503,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>132</v>
       </c>
@@ -1656,7 +1514,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>134</v>
       </c>
@@ -1667,7 +1525,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>136</v>
       </c>
@@ -1678,7 +1536,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>138</v>
       </c>
@@ -1689,7 +1547,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>140</v>
       </c>
@@ -1700,7 +1558,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>142</v>
       </c>
@@ -1711,7 +1569,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>144</v>
       </c>
@@ -1722,7 +1580,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>146</v>
       </c>
@@ -1733,7 +1591,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>148</v>
       </c>
@@ -1744,7 +1602,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>150</v>
       </c>
@@ -1755,7 +1613,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>152</v>
       </c>
@@ -1766,7 +1624,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>154</v>
       </c>
@@ -1777,7 +1635,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>156</v>
       </c>
@@ -1788,7 +1646,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>158</v>
       </c>
@@ -1799,7 +1657,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>160</v>
       </c>
@@ -1810,7 +1668,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>162</v>
       </c>
@@ -1821,7 +1679,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>164</v>
       </c>
@@ -1832,7 +1690,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>166</v>
       </c>
@@ -1843,7 +1701,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>168</v>
       </c>
@@ -1854,7 +1712,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>170</v>
       </c>
@@ -1865,7 +1723,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>172</v>
       </c>
@@ -1876,7 +1734,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>174</v>
       </c>
@@ -1887,7 +1745,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>176</v>
       </c>
@@ -1898,7 +1756,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>178</v>
       </c>
@@ -1909,7 +1767,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>180</v>
       </c>
@@ -1920,7 +1778,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>47</v>
       </c>
@@ -1931,7 +1789,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>50</v>
       </c>
@@ -1942,7 +1800,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>52</v>
       </c>
@@ -1953,7 +1811,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>185</v>
       </c>
@@ -1964,7 +1822,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>187</v>
       </c>
@@ -1975,7 +1833,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>189</v>
       </c>
@@ -1986,7 +1844,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>191</v>
       </c>

</xml_diff>